<commit_message>
Project state when running bin size tests for maxbin.
</commit_message>
<xml_diff>
--- a/results/Results Table.xlsx
+++ b/results/Results Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikim\Local Work--Not Uploaded\Thesis\Volleyball\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6AB260-DB71-4118-92E0-543E9F6725C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF0F15F-15B2-45B1-B482-56C428212D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BB76F719-0AF5-48F9-86C0-2961CA8A5D9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>W+L</t>
   </si>
@@ -137,18 +137,27 @@
   <si>
     <t>25 bin l w</t>
   </si>
+  <si>
+    <t> 0.6935786435786435</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFD1D2D3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,8 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,10 +955,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$G$27:$U$27</c:f>
+              <c:f>Sheet1!$G$27:$AK$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -993,16 +1003,64 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$28:$U$28</c:f>
+              <c:f>Sheet1!$G$28:$AK$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0.86799968194687904</c:v>
                 </c:pt>
@@ -1047,6 +1105,54 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.87726675425863498</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.86613605945832295</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86063168743160701</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85441336330312101</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85062206077064295</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.83659504559782305</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.82520107634398798</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.81174896390206497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.81316543180428502</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.80435261614186304</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.80971360382225899</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.80751781644793896</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.81102567908013401</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.81049891113696304</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.80678549602815497</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.81179996617519601</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.80819315049442397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3983,16 +4089,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4055,16 +4161,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4091,16 +4197,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4425,10 +4531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8100C0-3AD5-403E-B69E-FDFD72876661}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31:J32"/>
+    <sheetView tabSelected="1" topLeftCell="O7" workbookViewId="0">
+      <selection activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4647,7 +4753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -4676,7 +4782,7 @@
         <v>0.81031249316895004</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -4693,7 +4799,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -4704,7 +4810,7 @@
         <v>0.99993872173539999</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -4715,7 +4821,7 @@
         <v>0.99993857999600899</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -4726,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -4737,7 +4843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -4748,7 +4854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -4762,7 +4868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -4820,8 +4926,56 @@
       <c r="U27">
         <v>75</v>
       </c>
+      <c r="V27">
+        <v>90</v>
+      </c>
+      <c r="W27">
+        <v>110</v>
+      </c>
+      <c r="X27">
+        <v>130</v>
+      </c>
+      <c r="Y27">
+        <v>150</v>
+      </c>
+      <c r="Z27">
+        <v>170</v>
+      </c>
+      <c r="AA27">
+        <v>190</v>
+      </c>
+      <c r="AB27">
+        <v>210</v>
+      </c>
+      <c r="AC27">
+        <v>230</v>
+      </c>
+      <c r="AD27">
+        <v>250</v>
+      </c>
+      <c r="AE27">
+        <v>270</v>
+      </c>
+      <c r="AF27">
+        <v>290</v>
+      </c>
+      <c r="AG27">
+        <v>310</v>
+      </c>
+      <c r="AH27">
+        <v>330</v>
+      </c>
+      <c r="AI27">
+        <v>350</v>
+      </c>
+      <c r="AJ27">
+        <v>370</v>
+      </c>
+      <c r="AK27">
+        <v>390</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>26</v>
       </c>
@@ -4870,8 +5024,56 @@
       <c r="U28">
         <v>0.87726675425863498</v>
       </c>
+      <c r="V28">
+        <v>0.86613605945832295</v>
+      </c>
+      <c r="W28">
+        <v>0.86063168743160701</v>
+      </c>
+      <c r="X28">
+        <v>0.85441336330312101</v>
+      </c>
+      <c r="Y28">
+        <v>0.85062206077064295</v>
+      </c>
+      <c r="Z28">
+        <v>0.83659504559782305</v>
+      </c>
+      <c r="AA28">
+        <v>0.82520107634398798</v>
+      </c>
+      <c r="AB28">
+        <v>0.81174896390206497</v>
+      </c>
+      <c r="AC28">
+        <v>0.81316543180428502</v>
+      </c>
+      <c r="AD28">
+        <v>0.80435261614186304</v>
+      </c>
+      <c r="AE28">
+        <v>0.80971360382225899</v>
+      </c>
+      <c r="AF28">
+        <v>0.80751781644793896</v>
+      </c>
+      <c r="AG28">
+        <v>0.81102567908013401</v>
+      </c>
+      <c r="AH28">
+        <v>0.81049891113696304</v>
+      </c>
+      <c r="AI28">
+        <v>0.80678549602815497</v>
+      </c>
+      <c r="AJ28">
+        <v>0.81179996617519601</v>
+      </c>
+      <c r="AK28">
+        <v>0.80819315049442397</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -4879,7 +5081,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -4890,7 +5092,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4913,7 +5115,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>26</v>
       </c>
@@ -4930,12 +5132,12 @@
         <v>0.88343269164395699</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -4943,12 +5145,12 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -4956,12 +5158,12 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -4969,17 +5171,39 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="1">
+        <v>0.70440657827021402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>29</v>
       </c>
+      <c r="H44" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
       <c r="B45">
         <v>0.88</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.61670438147710804</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="1">
+        <v>0.56640348288075504</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <f>AVERAGE(H43:H46)</f>
+        <v>0.6291714808760257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project state when running bin size tests for sensor location.
</commit_message>
<xml_diff>
--- a/results/Results Table.xlsx
+++ b/results/Results Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikim\Local Work--Not Uploaded\Thesis\Volleyball\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF0F15F-15B2-45B1-B482-56C428212D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15110F6B-B262-48E2-B008-05DE0C51C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BB76F719-0AF5-48F9-86C0-2961CA8A5D9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>W+L</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t> 0.6935786435786435</t>
+  </si>
+  <si>
+    <t>new sensor location experiment</t>
+  </si>
+  <si>
+    <t>400, 50, maxmag</t>
+  </si>
+  <si>
+    <t>W L</t>
+  </si>
+  <si>
+    <t>W R</t>
+  </si>
+  <si>
+    <t>R L</t>
   </si>
 </sst>
 </file>
@@ -4198,15 +4213,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4533,8 +4548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8100C0-3AD5-403E-B69E-FDFD72876661}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O7" workbookViewId="0">
-      <selection activeCell="AK28" sqref="AK28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5132,12 +5147,12 @@
         <v>0.88343269164395699</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -5145,25 +5160,104 @@
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>27</v>
       </c>
+      <c r="F38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38" t="s">
+        <v>39</v>
+      </c>
+      <c r="M38" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
       <c r="B39">
         <v>0.82</v>
       </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39">
+        <v>0.81916067969252504</v>
+      </c>
+      <c r="H39">
+        <v>0.85101199171269004</v>
+      </c>
+      <c r="I39">
+        <v>0.81825354459291699</v>
+      </c>
+      <c r="J39">
+        <v>0.88158911832264197</v>
+      </c>
+      <c r="K39">
+        <v>0.87687349263494896</v>
+      </c>
+      <c r="L39">
+        <v>0.91159276762340302</v>
+      </c>
+      <c r="M39">
+        <v>0.916500755539568</v>
+      </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40">
+        <v>0.85775351128751598</v>
+      </c>
+      <c r="H40">
+        <v>0.90739485123363395</v>
+      </c>
+      <c r="I40">
+        <v>0.88217792117237903</v>
+      </c>
+      <c r="J40">
+        <v>0.91170816872625104</v>
+      </c>
+      <c r="K40">
+        <v>0.92854280278030998</v>
+      </c>
+      <c r="L40">
+        <v>0.95385457966846099</v>
+      </c>
+      <c r="M40">
+        <v>0.95285580712696105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -5171,12 +5265,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H43" s="1">
         <v>0.70440657827021402</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -5184,7 +5278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -5195,12 +5289,12 @@
         <v>0.61670438147710804</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H46" s="1">
         <v>0.56640348288075504</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H47">
         <f>AVERAGE(H43:H46)</f>
         <v>0.6291714808760257</v>

</xml_diff>

<commit_message>
Add preprocess_script.py, writing results
</commit_message>
<xml_diff>
--- a/results/Results Table.xlsx
+++ b/results/Results Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikim\Local Work--Not Uploaded\Thesis\Volleyball\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15110F6B-B262-48E2-B008-05DE0C51C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22FAC43-DB2A-47BD-B3B8-D422EE64510C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BB76F719-0AF5-48F9-86C0-2961CA8A5D9F}"/>
   </bookViews>
@@ -4549,7 +4549,7 @@
   <dimension ref="A1:AK47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>